<commit_message>
Automating the Input files for Transavia
</commit_message>
<xml_diff>
--- a/RAAL/Consumption/Input_Consumption_RAAL.xlsx
+++ b/RAAL/Consumption/Input_Consumption_RAAL.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mynexte-my.sharepoint.com/personal/andrei_ionita_mynexte_com/Documents/Desktop/ML/Forecast_app/RAAL/Consumption/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_23F921EDB0034F60D1644084E94C8FB6426863F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D114CAE4-1102-4F79-91D2-704DBCAFCD75}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -40,302 +34,302 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>23.02.202414</t>
-  </si>
-  <si>
-    <t>23.02.202415</t>
-  </si>
-  <si>
-    <t>23.02.202416</t>
-  </si>
-  <si>
-    <t>23.02.202417</t>
-  </si>
-  <si>
-    <t>23.02.202418</t>
-  </si>
-  <si>
-    <t>23.02.202419</t>
-  </si>
-  <si>
-    <t>23.02.202420</t>
-  </si>
-  <si>
-    <t>23.02.202421</t>
-  </si>
-  <si>
-    <t>23.02.202422</t>
-  </si>
-  <si>
-    <t>23.02.202423</t>
-  </si>
-  <si>
-    <t>24.02.20240</t>
-  </si>
-  <si>
-    <t>24.02.20241</t>
-  </si>
-  <si>
-    <t>24.02.20242</t>
-  </si>
-  <si>
-    <t>24.02.20243</t>
-  </si>
-  <si>
-    <t>24.02.20244</t>
-  </si>
-  <si>
-    <t>24.02.20245</t>
-  </si>
-  <si>
-    <t>24.02.20246</t>
-  </si>
-  <si>
-    <t>24.02.20247</t>
-  </si>
-  <si>
-    <t>24.02.20248</t>
-  </si>
-  <si>
-    <t>24.02.20249</t>
-  </si>
-  <si>
-    <t>24.02.202410</t>
-  </si>
-  <si>
-    <t>24.02.202411</t>
-  </si>
-  <si>
-    <t>24.02.202412</t>
-  </si>
-  <si>
-    <t>24.02.202413</t>
-  </si>
-  <si>
-    <t>24.02.202414</t>
-  </si>
-  <si>
-    <t>24.02.202415</t>
-  </si>
-  <si>
-    <t>24.02.202416</t>
-  </si>
-  <si>
-    <t>24.02.202417</t>
-  </si>
-  <si>
-    <t>24.02.202418</t>
-  </si>
-  <si>
-    <t>24.02.202419</t>
-  </si>
-  <si>
-    <t>24.02.202420</t>
-  </si>
-  <si>
-    <t>24.02.202421</t>
-  </si>
-  <si>
-    <t>24.02.202422</t>
-  </si>
-  <si>
-    <t>24.02.202423</t>
-  </si>
-  <si>
-    <t>25.02.20240</t>
-  </si>
-  <si>
-    <t>25.02.20241</t>
-  </si>
-  <si>
-    <t>25.02.20242</t>
-  </si>
-  <si>
-    <t>25.02.20243</t>
-  </si>
-  <si>
-    <t>25.02.20244</t>
-  </si>
-  <si>
-    <t>25.02.20245</t>
-  </si>
-  <si>
-    <t>25.02.20246</t>
-  </si>
-  <si>
-    <t>25.02.20247</t>
-  </si>
-  <si>
-    <t>25.02.20248</t>
-  </si>
-  <si>
-    <t>25.02.20249</t>
-  </si>
-  <si>
-    <t>25.02.202410</t>
-  </si>
-  <si>
-    <t>25.02.202411</t>
-  </si>
-  <si>
-    <t>25.02.202412</t>
-  </si>
-  <si>
-    <t>25.02.202413</t>
-  </si>
-  <si>
-    <t>25.02.202414</t>
-  </si>
-  <si>
-    <t>25.02.202415</t>
-  </si>
-  <si>
-    <t>25.02.202416</t>
-  </si>
-  <si>
-    <t>25.02.202417</t>
-  </si>
-  <si>
-    <t>25.02.202418</t>
-  </si>
-  <si>
-    <t>25.02.202419</t>
-  </si>
-  <si>
-    <t>25.02.202420</t>
-  </si>
-  <si>
-    <t>25.02.202421</t>
-  </si>
-  <si>
-    <t>25.02.202422</t>
-  </si>
-  <si>
-    <t>25.02.202423</t>
-  </si>
-  <si>
-    <t>26.02.20240</t>
-  </si>
-  <si>
-    <t>26.02.20241</t>
-  </si>
-  <si>
-    <t>26.02.20242</t>
-  </si>
-  <si>
-    <t>26.02.20243</t>
-  </si>
-  <si>
-    <t>26.02.20244</t>
-  </si>
-  <si>
-    <t>26.02.20245</t>
-  </si>
-  <si>
-    <t>26.02.20246</t>
-  </si>
-  <si>
-    <t>26.02.20247</t>
-  </si>
-  <si>
-    <t>26.02.20248</t>
-  </si>
-  <si>
-    <t>26.02.20249</t>
-  </si>
-  <si>
-    <t>26.02.202410</t>
-  </si>
-  <si>
-    <t>26.02.202411</t>
-  </si>
-  <si>
-    <t>26.02.202412</t>
-  </si>
-  <si>
-    <t>26.02.202413</t>
-  </si>
-  <si>
-    <t>26.02.202414</t>
-  </si>
-  <si>
-    <t>26.02.202415</t>
-  </si>
-  <si>
-    <t>26.02.202416</t>
-  </si>
-  <si>
-    <t>26.02.202417</t>
-  </si>
-  <si>
-    <t>26.02.202418</t>
-  </si>
-  <si>
-    <t>26.02.202419</t>
-  </si>
-  <si>
-    <t>26.02.202420</t>
-  </si>
-  <si>
-    <t>26.02.202421</t>
-  </si>
-  <si>
-    <t>26.02.202422</t>
-  </si>
-  <si>
-    <t>26.02.202423</t>
-  </si>
-  <si>
-    <t>27.02.20240</t>
-  </si>
-  <si>
-    <t>27.02.20241</t>
-  </si>
-  <si>
-    <t>27.02.20242</t>
-  </si>
-  <si>
-    <t>27.02.20243</t>
-  </si>
-  <si>
-    <t>27.02.20244</t>
-  </si>
-  <si>
-    <t>27.02.20245</t>
-  </si>
-  <si>
-    <t>27.02.20246</t>
-  </si>
-  <si>
-    <t>27.02.20247</t>
-  </si>
-  <si>
-    <t>27.02.20248</t>
-  </si>
-  <si>
-    <t>27.02.20249</t>
-  </si>
-  <si>
-    <t>27.02.202410</t>
-  </si>
-  <si>
-    <t>27.02.202411</t>
-  </si>
-  <si>
-    <t>27.02.202412</t>
-  </si>
-  <si>
-    <t>27.02.202413</t>
+    <t>19.03.202410</t>
+  </si>
+  <si>
+    <t>19.03.202411</t>
+  </si>
+  <si>
+    <t>19.03.202412</t>
+  </si>
+  <si>
+    <t>19.03.202413</t>
+  </si>
+  <si>
+    <t>19.03.202414</t>
+  </si>
+  <si>
+    <t>19.03.202415</t>
+  </si>
+  <si>
+    <t>19.03.202416</t>
+  </si>
+  <si>
+    <t>19.03.202417</t>
+  </si>
+  <si>
+    <t>19.03.202418</t>
+  </si>
+  <si>
+    <t>19.03.202419</t>
+  </si>
+  <si>
+    <t>19.03.202420</t>
+  </si>
+  <si>
+    <t>19.03.202421</t>
+  </si>
+  <si>
+    <t>19.03.202422</t>
+  </si>
+  <si>
+    <t>19.03.202423</t>
+  </si>
+  <si>
+    <t>20.03.20240</t>
+  </si>
+  <si>
+    <t>20.03.20241</t>
+  </si>
+  <si>
+    <t>20.03.20242</t>
+  </si>
+  <si>
+    <t>20.03.20243</t>
+  </si>
+  <si>
+    <t>20.03.20244</t>
+  </si>
+  <si>
+    <t>20.03.20245</t>
+  </si>
+  <si>
+    <t>20.03.20246</t>
+  </si>
+  <si>
+    <t>20.03.20247</t>
+  </si>
+  <si>
+    <t>20.03.20248</t>
+  </si>
+  <si>
+    <t>20.03.20249</t>
+  </si>
+  <si>
+    <t>20.03.202410</t>
+  </si>
+  <si>
+    <t>20.03.202411</t>
+  </si>
+  <si>
+    <t>20.03.202412</t>
+  </si>
+  <si>
+    <t>20.03.202413</t>
+  </si>
+  <si>
+    <t>20.03.202414</t>
+  </si>
+  <si>
+    <t>20.03.202415</t>
+  </si>
+  <si>
+    <t>20.03.202416</t>
+  </si>
+  <si>
+    <t>20.03.202417</t>
+  </si>
+  <si>
+    <t>20.03.202418</t>
+  </si>
+  <si>
+    <t>20.03.202419</t>
+  </si>
+  <si>
+    <t>20.03.202420</t>
+  </si>
+  <si>
+    <t>20.03.202421</t>
+  </si>
+  <si>
+    <t>20.03.202422</t>
+  </si>
+  <si>
+    <t>20.03.202423</t>
+  </si>
+  <si>
+    <t>21.03.20240</t>
+  </si>
+  <si>
+    <t>21.03.20241</t>
+  </si>
+  <si>
+    <t>21.03.20242</t>
+  </si>
+  <si>
+    <t>21.03.20243</t>
+  </si>
+  <si>
+    <t>21.03.20244</t>
+  </si>
+  <si>
+    <t>21.03.20245</t>
+  </si>
+  <si>
+    <t>21.03.20246</t>
+  </si>
+  <si>
+    <t>21.03.20247</t>
+  </si>
+  <si>
+    <t>21.03.20248</t>
+  </si>
+  <si>
+    <t>21.03.20249</t>
+  </si>
+  <si>
+    <t>21.03.202410</t>
+  </si>
+  <si>
+    <t>21.03.202411</t>
+  </si>
+  <si>
+    <t>21.03.202412</t>
+  </si>
+  <si>
+    <t>21.03.202413</t>
+  </si>
+  <si>
+    <t>21.03.202414</t>
+  </si>
+  <si>
+    <t>21.03.202415</t>
+  </si>
+  <si>
+    <t>21.03.202416</t>
+  </si>
+  <si>
+    <t>21.03.202417</t>
+  </si>
+  <si>
+    <t>21.03.202418</t>
+  </si>
+  <si>
+    <t>21.03.202419</t>
+  </si>
+  <si>
+    <t>21.03.202420</t>
+  </si>
+  <si>
+    <t>21.03.202421</t>
+  </si>
+  <si>
+    <t>21.03.202422</t>
+  </si>
+  <si>
+    <t>21.03.202423</t>
+  </si>
+  <si>
+    <t>22.03.20240</t>
+  </si>
+  <si>
+    <t>22.03.20241</t>
+  </si>
+  <si>
+    <t>22.03.20242</t>
+  </si>
+  <si>
+    <t>22.03.20243</t>
+  </si>
+  <si>
+    <t>22.03.20244</t>
+  </si>
+  <si>
+    <t>22.03.20245</t>
+  </si>
+  <si>
+    <t>22.03.20246</t>
+  </si>
+  <si>
+    <t>22.03.20247</t>
+  </si>
+  <si>
+    <t>22.03.20248</t>
+  </si>
+  <si>
+    <t>22.03.20249</t>
+  </si>
+  <si>
+    <t>22.03.202410</t>
+  </si>
+  <si>
+    <t>22.03.202411</t>
+  </si>
+  <si>
+    <t>22.03.202412</t>
+  </si>
+  <si>
+    <t>22.03.202413</t>
+  </si>
+  <si>
+    <t>22.03.202414</t>
+  </si>
+  <si>
+    <t>22.03.202415</t>
+  </si>
+  <si>
+    <t>22.03.202416</t>
+  </si>
+  <si>
+    <t>22.03.202417</t>
+  </si>
+  <si>
+    <t>22.03.202418</t>
+  </si>
+  <si>
+    <t>22.03.202419</t>
+  </si>
+  <si>
+    <t>22.03.202420</t>
+  </si>
+  <si>
+    <t>22.03.202421</t>
+  </si>
+  <si>
+    <t>22.03.202422</t>
+  </si>
+  <si>
+    <t>22.03.202423</t>
+  </si>
+  <si>
+    <t>23.03.20240</t>
+  </si>
+  <si>
+    <t>23.03.20241</t>
+  </si>
+  <si>
+    <t>23.03.20242</t>
+  </si>
+  <si>
+    <t>23.03.20243</t>
+  </si>
+  <si>
+    <t>23.03.20244</t>
+  </si>
+  <si>
+    <t>23.03.20245</t>
+  </si>
+  <si>
+    <t>23.03.20246</t>
+  </si>
+  <si>
+    <t>23.03.20247</t>
+  </si>
+  <si>
+    <t>23.03.20248</t>
+  </si>
+  <si>
+    <t>23.03.20249</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,21 +393,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -451,7 +437,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -485,7 +471,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -520,10 +505,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -696,19 +680,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="R20" sqref="R19:R20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -728,572 +707,578 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
-        <v>45345</v>
+        <v>45370</v>
       </c>
       <c r="B2">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>110.27</v>
+        <v>538.4400000000001</v>
+      </c>
+      <c r="D2">
+        <v>5.43</v>
+      </c>
+      <c r="E2">
+        <v>71</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>45345</v>
+        <v>45370</v>
       </c>
       <c r="B3">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C3">
-        <v>81.77</v>
+        <v>547.02</v>
       </c>
       <c r="D3">
-        <v>10.98</v>
+        <v>5.44</v>
       </c>
       <c r="E3">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
-        <v>45345</v>
+        <v>45370</v>
       </c>
       <c r="B4">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>48.68</v>
+        <v>511.63</v>
       </c>
       <c r="D4">
-        <v>10.33</v>
+        <v>5.55</v>
       </c>
       <c r="E4">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
-        <v>45345</v>
+        <v>45370</v>
       </c>
       <c r="B5">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C5">
-        <v>11.24</v>
+        <v>448.1</v>
       </c>
       <c r="D5">
-        <v>9.42</v>
+        <v>5.89</v>
       </c>
       <c r="E5">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
-        <v>45345</v>
+        <v>45370</v>
       </c>
       <c r="B6">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>300.77</v>
       </c>
       <c r="D6">
-        <v>8.41</v>
+        <v>5.96</v>
       </c>
       <c r="E6">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
-        <v>45345</v>
+        <v>45370</v>
       </c>
       <c r="B7">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>116.76</v>
       </c>
       <c r="D7">
-        <v>7.4</v>
+        <v>5.43</v>
       </c>
       <c r="E7">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
-        <v>45345</v>
+        <v>45370</v>
       </c>
       <c r="B8">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>75.22</v>
       </c>
       <c r="D8">
-        <v>6.1</v>
+        <v>4.04</v>
       </c>
       <c r="E8">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="F8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="2">
-        <v>45345</v>
+        <v>45370</v>
       </c>
       <c r="B9">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>33.25</v>
       </c>
       <c r="D9">
-        <v>5.89</v>
+        <v>2.15</v>
       </c>
       <c r="E9">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="F9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="2">
-        <v>45345</v>
+        <v>45370</v>
       </c>
       <c r="B10">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>2.65</v>
       </c>
       <c r="D10">
-        <v>5.76</v>
+        <v>1.31</v>
       </c>
       <c r="E10">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="2">
-        <v>45345</v>
+        <v>45370</v>
       </c>
       <c r="B11">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>5.6</v>
+        <v>1.08</v>
       </c>
       <c r="E11">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="2">
-        <v>45346</v>
+        <v>45370</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>5.41</v>
+        <v>0.74</v>
       </c>
       <c r="E12">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="F12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="2">
-        <v>45346</v>
+        <v>45370</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>5.27</v>
+        <v>0.57</v>
       </c>
       <c r="E13">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="2">
-        <v>45346</v>
+        <v>45370</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>5.0999999999999996</v>
+        <v>0.55</v>
       </c>
       <c r="E14">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="F14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="2">
-        <v>45346</v>
+        <v>45370</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>4.96</v>
+        <v>0.49</v>
       </c>
       <c r="E15">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="F15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="2">
-        <v>45346</v>
+        <v>45371</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>4.97</v>
+        <v>0.55</v>
       </c>
       <c r="E16">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="2">
-        <v>45346</v>
+        <v>45371</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>5.37</v>
+        <v>0.33</v>
       </c>
       <c r="E17">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="F17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="2">
-        <v>45346</v>
+        <v>45371</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>6.03</v>
+        <v>0.25</v>
       </c>
       <c r="E18">
-        <v>90</v>
+        <v>27</v>
       </c>
       <c r="F18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="2">
-        <v>45346</v>
+        <v>45371</v>
       </c>
       <c r="B19">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>12.03</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>8.16</v>
+        <v>0.16</v>
       </c>
       <c r="E19">
-        <v>98</v>
+        <v>26</v>
       </c>
       <c r="F19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="2">
-        <v>45346</v>
+        <v>45371</v>
       </c>
       <c r="B20">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C20">
-        <v>62.55</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>10.199999999999999</v>
+        <v>-0.01</v>
       </c>
       <c r="E20">
-        <v>99</v>
+        <v>29</v>
       </c>
       <c r="F20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="2">
-        <v>45346</v>
+        <v>45371</v>
       </c>
       <c r="B21">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C21">
-        <v>91.11</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>11.4</v>
+        <v>0.29</v>
       </c>
       <c r="E21">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="F21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="2">
-        <v>45346</v>
+        <v>45371</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C22">
-        <v>120.44</v>
+        <v>12.26</v>
       </c>
       <c r="D22">
-        <v>11.96</v>
+        <v>1.7</v>
       </c>
       <c r="E22">
-        <v>99</v>
+        <v>38</v>
       </c>
       <c r="F22" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="2">
-        <v>45346</v>
+        <v>45371</v>
       </c>
       <c r="B23">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C23">
-        <v>138.96</v>
+        <v>132.49</v>
       </c>
       <c r="D23">
-        <v>12.35</v>
+        <v>3.11</v>
       </c>
       <c r="E23">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="F23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="2">
-        <v>45346</v>
+        <v>45371</v>
       </c>
       <c r="B24">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C24">
-        <v>144.51</v>
+        <v>274.71</v>
       </c>
       <c r="D24">
-        <v>12.68</v>
+        <v>4.38</v>
       </c>
       <c r="E24">
-        <v>100</v>
+        <v>71</v>
       </c>
       <c r="F24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="2">
-        <v>45346</v>
+        <v>45371</v>
       </c>
       <c r="B25">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C25">
-        <v>136.69</v>
+        <v>348.56</v>
       </c>
       <c r="D25">
-        <v>12.81</v>
+        <v>5.35</v>
       </c>
       <c r="E25">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="F25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="2">
-        <v>45346</v>
+        <v>45371</v>
       </c>
       <c r="B26">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C26">
-        <v>114.44</v>
+        <v>440.57</v>
       </c>
       <c r="D26">
-        <v>12.55</v>
+        <v>5.94</v>
       </c>
       <c r="E26">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="F26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="2">
-        <v>45346</v>
+        <v>45371</v>
       </c>
       <c r="B27">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C27">
-        <v>81.72</v>
+        <v>470.06</v>
       </c>
       <c r="D27">
-        <v>11.36</v>
+        <v>6.37</v>
       </c>
       <c r="E27">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="F27" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="2">
-        <v>45346</v>
+        <v>45371</v>
       </c>
       <c r="B28">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C28">
-        <v>45.12</v>
+        <v>480.86</v>
       </c>
       <c r="D28">
-        <v>10.26</v>
+        <v>6.03</v>
       </c>
       <c r="E28">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F28" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="2">
-        <v>45346</v>
+        <v>45371</v>
       </c>
       <c r="B29">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C29">
-        <v>9.77</v>
+        <v>455.1</v>
       </c>
       <c r="D29">
-        <v>9.8000000000000007</v>
+        <v>5.65</v>
       </c>
       <c r="E29">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F29" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="2">
-        <v>45346</v>
+        <v>45371</v>
       </c>
       <c r="B30">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>308.69</v>
       </c>
       <c r="D30">
-        <v>9.4700000000000006</v>
+        <v>5.44</v>
       </c>
       <c r="E30">
         <v>100</v>
@@ -1302,18 +1287,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="2">
-        <v>45346</v>
+        <v>45371</v>
       </c>
       <c r="B31">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>122.24</v>
       </c>
       <c r="D31">
-        <v>9.18</v>
+        <v>5.7</v>
       </c>
       <c r="E31">
         <v>100</v>
@@ -1322,598 +1307,598 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="2">
-        <v>45346</v>
+        <v>45371</v>
       </c>
       <c r="B32">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>77.62</v>
       </c>
       <c r="D32">
-        <v>9.23</v>
+        <v>5.03</v>
       </c>
       <c r="E32">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F32" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="2">
-        <v>45346</v>
+        <v>45371</v>
       </c>
       <c r="B33">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>35.78</v>
       </c>
       <c r="D33">
-        <v>9.32</v>
+        <v>3.32</v>
       </c>
       <c r="E33">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F33" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="2">
-        <v>45346</v>
+        <v>45371</v>
       </c>
       <c r="B34">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>3.41</v>
       </c>
       <c r="D34">
-        <v>9.3000000000000007</v>
+        <v>2.42</v>
       </c>
       <c r="E34">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="F34" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="2">
-        <v>45346</v>
+        <v>45371</v>
       </c>
       <c r="B35">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
-        <v>9.4</v>
+        <v>1.72</v>
       </c>
       <c r="E35">
-        <v>100</v>
+        <v>38</v>
       </c>
       <c r="F35" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" s="2">
-        <v>45347</v>
+        <v>45371</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
-        <v>9.2899999999999991</v>
+        <v>1.73</v>
       </c>
       <c r="E36">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="F36" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="2">
-        <v>45347</v>
+        <v>45371</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
-        <v>9.24</v>
+        <v>2.28</v>
       </c>
       <c r="E37">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="F37" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" s="2">
-        <v>45347</v>
+        <v>45371</v>
       </c>
       <c r="B38">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>9.0399999999999991</v>
+        <v>2.34</v>
       </c>
       <c r="E38">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="F38" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" s="2">
-        <v>45347</v>
+        <v>45371</v>
       </c>
       <c r="B39">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
-        <v>8.2799999999999994</v>
+        <v>1.7</v>
       </c>
       <c r="E39">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="F39" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40" s="2">
-        <v>45347</v>
+        <v>45372</v>
       </c>
       <c r="B40">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40">
-        <v>7.99</v>
+        <v>0.58</v>
       </c>
       <c r="E40">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="F40" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" s="2">
-        <v>45347</v>
+        <v>45372</v>
       </c>
       <c r="B41">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41">
-        <v>7.75</v>
+        <v>0.03</v>
       </c>
       <c r="E41">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="F41" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="2">
-        <v>45347</v>
+        <v>45372</v>
       </c>
       <c r="B42">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42">
-        <v>8.18</v>
+        <v>-0.39</v>
       </c>
       <c r="E42">
-        <v>100</v>
+        <v>34</v>
       </c>
       <c r="F42" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43" s="2">
-        <v>45347</v>
+        <v>45372</v>
       </c>
       <c r="B43">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C43">
-        <v>6.9</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>9.5</v>
+        <v>-0.57</v>
       </c>
       <c r="E43">
-        <v>100</v>
+        <v>29</v>
       </c>
       <c r="F43" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44" s="2">
-        <v>45347</v>
+        <v>45372</v>
       </c>
       <c r="B44">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C44">
-        <v>40.47</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>11.16</v>
+        <v>-0.6899999999999999</v>
       </c>
       <c r="E44">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="F44" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" s="2">
-        <v>45347</v>
+        <v>45372</v>
       </c>
       <c r="B45">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C45">
-        <v>77.83</v>
+        <v>0</v>
       </c>
       <c r="D45">
-        <v>12.5</v>
+        <v>-0.2</v>
       </c>
       <c r="E45">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="F45" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46" s="2">
-        <v>45347</v>
+        <v>45372</v>
       </c>
       <c r="B46">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C46">
-        <v>108.86</v>
+        <v>14.22</v>
       </c>
       <c r="D46">
-        <v>13.52</v>
+        <v>1.98</v>
       </c>
       <c r="E46">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="F46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47" s="2">
-        <v>45347</v>
+        <v>45372</v>
       </c>
       <c r="B47">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C47">
-        <v>129.41999999999999</v>
+        <v>140.19</v>
       </c>
       <c r="D47">
-        <v>14.16</v>
+        <v>4.14</v>
       </c>
       <c r="E47">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="F47" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48" s="2">
-        <v>45347</v>
+        <v>45372</v>
       </c>
       <c r="B48">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C48">
-        <v>137.22</v>
+        <v>309.91</v>
       </c>
       <c r="D48">
-        <v>14.13</v>
+        <v>5.84</v>
       </c>
       <c r="E48">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="F48" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49" s="2">
-        <v>45347</v>
+        <v>45372</v>
       </c>
       <c r="B49">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C49">
-        <v>131.44999999999999</v>
+        <v>468.29</v>
       </c>
       <c r="D49">
-        <v>13.97</v>
+        <v>6.92</v>
       </c>
       <c r="E49">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="F49" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" s="2">
-        <v>45347</v>
+        <v>45372</v>
       </c>
       <c r="B50">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C50">
-        <v>112.71</v>
+        <v>593.79</v>
       </c>
       <c r="D50">
-        <v>13.27</v>
+        <v>7.81</v>
       </c>
       <c r="E50">
-        <v>100</v>
+        <v>7</v>
       </c>
       <c r="F50" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="A51" s="2">
-        <v>45347</v>
+        <v>45372</v>
       </c>
       <c r="B51">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C51">
-        <v>83.06</v>
+        <v>673.63</v>
       </c>
       <c r="D51">
-        <v>12.05</v>
+        <v>8.390000000000001</v>
       </c>
       <c r="E51">
-        <v>100</v>
+        <v>7</v>
       </c>
       <c r="F51" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" s="2">
-        <v>45347</v>
+        <v>45372</v>
       </c>
       <c r="B52">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C52">
-        <v>46.3</v>
+        <v>700.1</v>
       </c>
       <c r="D52">
-        <v>11.13</v>
+        <v>8.83</v>
       </c>
       <c r="E52">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="F52" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="2">
-        <v>45347</v>
+        <v>45372</v>
       </c>
       <c r="B53">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C53">
-        <v>10.42</v>
+        <v>670.71</v>
       </c>
       <c r="D53">
-        <v>10.8</v>
+        <v>9.17</v>
       </c>
       <c r="E53">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="F53" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="A54" s="2">
-        <v>45347</v>
+        <v>45372</v>
       </c>
       <c r="B54">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>577.49</v>
       </c>
       <c r="D54">
-        <v>10.45</v>
+        <v>9.279999999999999</v>
       </c>
       <c r="E54">
-        <v>100</v>
+        <v>38</v>
       </c>
       <c r="F54" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="A55" s="2">
-        <v>45347</v>
+        <v>45372</v>
       </c>
       <c r="B55">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>421.41</v>
       </c>
       <c r="D55">
-        <v>10.27</v>
+        <v>8.73</v>
       </c>
       <c r="E55">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="F55" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="A56" s="2">
-        <v>45347</v>
+        <v>45372</v>
       </c>
       <c r="B56">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>294.4</v>
       </c>
       <c r="D56">
-        <v>9.99</v>
+        <v>6.59</v>
       </c>
       <c r="E56">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="F56" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="A57" s="2">
-        <v>45347</v>
+        <v>45372</v>
       </c>
       <c r="B57">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>130.67</v>
       </c>
       <c r="D57">
-        <v>9.7100000000000009</v>
+        <v>4.17</v>
       </c>
       <c r="E57">
-        <v>100</v>
+        <v>28</v>
       </c>
       <c r="F57" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58" s="2">
-        <v>45347</v>
+        <v>45372</v>
       </c>
       <c r="B58">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>11.47</v>
       </c>
       <c r="D58">
-        <v>9.5299999999999994</v>
+        <v>3.44</v>
       </c>
       <c r="E58">
-        <v>100</v>
+        <v>38</v>
       </c>
       <c r="F58" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59" s="2">
-        <v>45347</v>
+        <v>45372</v>
       </c>
       <c r="B59">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
       <c r="D59">
-        <v>8.6999999999999993</v>
+        <v>2.99</v>
       </c>
       <c r="E59">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F59" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="A60" s="2">
-        <v>45348</v>
+        <v>45372</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
       <c r="D60">
-        <v>8.34</v>
+        <v>2.83</v>
       </c>
       <c r="E60">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F60" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61" s="2">
-        <v>45348</v>
+        <v>45372</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
       <c r="D61">
-        <v>8.69</v>
+        <v>2.6</v>
       </c>
       <c r="E61">
         <v>100</v>
@@ -1922,506 +1907,518 @@
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="A62" s="2">
-        <v>45348</v>
+        <v>45372</v>
       </c>
       <c r="B62">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
       <c r="D62">
-        <v>8.19</v>
+        <v>2.42</v>
       </c>
       <c r="E62">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F62" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="A63" s="2">
-        <v>45348</v>
+        <v>45372</v>
       </c>
       <c r="B63">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
       <c r="D63">
-        <v>7.52</v>
+        <v>2.27</v>
       </c>
       <c r="E63">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F63" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="A64" s="2">
-        <v>45348</v>
+        <v>45373</v>
       </c>
       <c r="B64">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C64">
         <v>0</v>
       </c>
       <c r="D64">
-        <v>7.21</v>
+        <v>2.17</v>
       </c>
       <c r="E64">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F64" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6">
       <c r="A65" s="2">
-        <v>45348</v>
+        <v>45373</v>
       </c>
       <c r="B65">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C65">
         <v>0</v>
       </c>
       <c r="D65">
-        <v>6.98</v>
+        <v>2.21</v>
       </c>
       <c r="E65">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="F65" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6">
       <c r="A66" s="2">
-        <v>45348</v>
+        <v>45373</v>
       </c>
       <c r="B66">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C66">
         <v>0</v>
       </c>
       <c r="D66">
-        <v>7.47</v>
+        <v>2.39</v>
       </c>
       <c r="E66">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="F66" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6">
       <c r="A67" s="2">
-        <v>45348</v>
+        <v>45373</v>
       </c>
       <c r="B67">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C67">
-        <v>15.62</v>
+        <v>0</v>
       </c>
       <c r="D67">
-        <v>9.7799999999999994</v>
+        <v>2.55</v>
       </c>
       <c r="E67">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="F67" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6">
       <c r="A68" s="2">
-        <v>45348</v>
+        <v>45373</v>
       </c>
       <c r="B68">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C68">
-        <v>109.41</v>
+        <v>0</v>
       </c>
       <c r="D68">
-        <v>11.91</v>
+        <v>2.58</v>
       </c>
       <c r="E68">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="F68" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6">
       <c r="A69" s="2">
-        <v>45348</v>
+        <v>45373</v>
       </c>
       <c r="B69">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C69">
-        <v>211.29</v>
+        <v>0</v>
       </c>
       <c r="D69">
-        <v>13.6</v>
+        <v>3</v>
       </c>
       <c r="E69">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="F69" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6">
       <c r="A70" s="2">
-        <v>45348</v>
+        <v>45373</v>
       </c>
       <c r="B70">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C70">
-        <v>226.94</v>
+        <v>4.09</v>
       </c>
       <c r="D70">
-        <v>14.93</v>
+        <v>3.93</v>
       </c>
       <c r="E70">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="F70" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6">
       <c r="A71" s="2">
-        <v>45348</v>
+        <v>45373</v>
       </c>
       <c r="B71">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C71">
-        <v>262.33999999999997</v>
+        <v>36.66</v>
       </c>
       <c r="D71">
-        <v>15.55</v>
+        <v>5.42</v>
       </c>
       <c r="E71">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="F71" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6">
       <c r="A72" s="2">
-        <v>45348</v>
+        <v>45373</v>
       </c>
       <c r="B72">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C72">
-        <v>319.37</v>
+        <v>79.2</v>
       </c>
       <c r="D72">
-        <v>15.98</v>
+        <v>6.97</v>
       </c>
       <c r="E72">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="F72" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6">
       <c r="A73" s="2">
-        <v>45348</v>
+        <v>45373</v>
       </c>
       <c r="B73">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C73">
-        <v>331.76</v>
+        <v>118.7</v>
       </c>
       <c r="D73">
-        <v>16.2</v>
+        <v>8.460000000000001</v>
       </c>
       <c r="E73">
-        <v>33</v>
+        <v>96</v>
       </c>
       <c r="F73" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6">
       <c r="A74" s="2">
-        <v>45348</v>
+        <v>45373</v>
       </c>
       <c r="B74">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C74">
-        <v>369.91</v>
+        <v>175.42</v>
       </c>
       <c r="D74">
-        <v>16.02</v>
+        <v>9.33</v>
       </c>
       <c r="E74">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="F74" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6">
       <c r="A75" s="2">
-        <v>45348</v>
+        <v>45373</v>
       </c>
       <c r="B75">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C75">
-        <v>330.5</v>
+        <v>287.62</v>
       </c>
       <c r="D75">
-        <v>14.67</v>
+        <v>9.890000000000001</v>
       </c>
       <c r="E75">
-        <v>34</v>
+        <v>73</v>
       </c>
       <c r="F75" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6">
       <c r="A76" s="2">
-        <v>45348</v>
+        <v>45373</v>
       </c>
       <c r="B76">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C76">
-        <v>184.99</v>
+        <v>432.36</v>
       </c>
       <c r="D76">
-        <v>12.14</v>
+        <v>10.08</v>
       </c>
       <c r="E76">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="F76" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6">
       <c r="A77" s="2">
-        <v>45348</v>
+        <v>45373</v>
       </c>
       <c r="B77">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C77">
-        <v>44.05</v>
+        <v>526</v>
       </c>
       <c r="D77">
-        <v>11.27</v>
+        <v>10.17</v>
       </c>
       <c r="E77">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="F77" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6">
       <c r="A78" s="2">
-        <v>45348</v>
+        <v>45373</v>
       </c>
       <c r="B78">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>541.79</v>
       </c>
       <c r="D78">
-        <v>10.65</v>
+        <v>9.82</v>
       </c>
       <c r="E78">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="F78" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6">
       <c r="A79" s="2">
-        <v>45348</v>
+        <v>45373</v>
       </c>
       <c r="B79">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>461.62</v>
       </c>
       <c r="D79">
-        <v>10.07</v>
+        <v>8.890000000000001</v>
       </c>
       <c r="E79">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F79" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6">
       <c r="A80" s="2">
-        <v>45348</v>
+        <v>45373</v>
       </c>
       <c r="B80">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>303.74</v>
       </c>
       <c r="D80">
-        <v>9.5399999999999991</v>
+        <v>7.02</v>
       </c>
       <c r="E80">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F80" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6">
       <c r="A81" s="2">
-        <v>45348</v>
+        <v>45373</v>
       </c>
       <c r="B81">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>135.59</v>
       </c>
       <c r="D81">
-        <v>9.01</v>
+        <v>4.55</v>
       </c>
       <c r="E81">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F81" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6">
       <c r="A82" s="2">
-        <v>45348</v>
+        <v>45373</v>
       </c>
       <c r="B82">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>12.79</v>
       </c>
       <c r="D82">
-        <v>8.58</v>
+        <v>3.38</v>
       </c>
       <c r="E82">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F82" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6">
       <c r="A83" s="2">
-        <v>45348</v>
+        <v>45373</v>
       </c>
       <c r="B83">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C83">
         <v>0</v>
       </c>
       <c r="D83">
-        <v>8.16</v>
+        <v>2.68</v>
       </c>
       <c r="E83">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F83" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6">
       <c r="A84" s="2">
-        <v>45349</v>
+        <v>45373</v>
       </c>
       <c r="B84">
+        <v>20</v>
+      </c>
+      <c r="C84">
         <v>0</v>
       </c>
       <c r="D84">
-        <v>7.79</v>
+        <v>2.27</v>
       </c>
       <c r="E84">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="F84" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6">
       <c r="A85" s="2">
-        <v>45349</v>
+        <v>45373</v>
       </c>
       <c r="B85">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
       </c>
       <c r="D85">
-        <v>7.43</v>
+        <v>1.94</v>
       </c>
       <c r="E85">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F85" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6">
       <c r="A86" s="2">
-        <v>45349</v>
+        <v>45373</v>
       </c>
       <c r="B86">
-        <v>2</v>
+        <v>22</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
       </c>
       <c r="D86">
-        <v>7.09</v>
+        <v>1.73</v>
       </c>
       <c r="E86">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F86" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6">
       <c r="A87" s="2">
-        <v>45349</v>
+        <v>45373</v>
       </c>
       <c r="B87">
-        <v>3</v>
+        <v>23</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
       </c>
       <c r="D87">
-        <v>6.85</v>
+        <v>1.46</v>
       </c>
       <c r="E87">
         <v>28</v>
@@ -2430,171 +2427,201 @@
         <v>91</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6">
       <c r="A88" s="2">
-        <v>45349</v>
+        <v>45374</v>
       </c>
       <c r="B88">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
       </c>
       <c r="D88">
-        <v>6.56</v>
+        <v>1.37</v>
       </c>
       <c r="E88">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F88" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6">
       <c r="A89" s="2">
-        <v>45349</v>
+        <v>45374</v>
       </c>
       <c r="B89">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
       </c>
       <c r="D89">
-        <v>6.19</v>
+        <v>2.14</v>
       </c>
       <c r="E89">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="F89" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6">
       <c r="A90" s="2">
-        <v>45349</v>
+        <v>45374</v>
       </c>
       <c r="B90">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
       </c>
       <c r="D90">
-        <v>6.9</v>
+        <v>2.51</v>
       </c>
       <c r="E90">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="F90" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6">
       <c r="A91" s="2">
-        <v>45349</v>
+        <v>45374</v>
       </c>
       <c r="B91">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
       </c>
       <c r="D91">
-        <v>9.42</v>
+        <v>2.43</v>
       </c>
       <c r="E91">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="F91" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6">
       <c r="A92" s="2">
-        <v>45349</v>
+        <v>45374</v>
       </c>
       <c r="B92">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
       </c>
       <c r="D92">
-        <v>11.71</v>
+        <v>1.17</v>
       </c>
       <c r="E92">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="F92" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6">
       <c r="A93" s="2">
-        <v>45349</v>
+        <v>45374</v>
       </c>
       <c r="B93">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
       </c>
       <c r="D93">
-        <v>13.46</v>
+        <v>1.64</v>
       </c>
       <c r="E93">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="F93" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6">
       <c r="A94" s="2">
-        <v>45349</v>
+        <v>45374</v>
       </c>
       <c r="B94">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="C94">
+        <v>15.77</v>
       </c>
       <c r="D94">
-        <v>14.37</v>
+        <v>4.01</v>
       </c>
       <c r="E94">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F94" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6">
       <c r="A95" s="2">
-        <v>45349</v>
+        <v>45374</v>
       </c>
       <c r="B95">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="C95">
+        <v>133.52</v>
       </c>
       <c r="D95">
-        <v>14.86</v>
+        <v>6.04</v>
       </c>
       <c r="E95">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="F95" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6">
       <c r="A96" s="2">
-        <v>45349</v>
+        <v>45374</v>
       </c>
       <c r="B96">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="C96">
+        <v>305.36</v>
       </c>
       <c r="D96">
-        <v>15.3</v>
+        <v>7.37</v>
       </c>
       <c r="E96">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="F96" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6">
       <c r="A97" s="2">
-        <v>45349</v>
+        <v>45374</v>
       </c>
       <c r="B97">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="C97">
+        <v>476.76</v>
       </c>
       <c r="D97">
-        <v>15.61</v>
+        <v>8.48</v>
       </c>
       <c r="E97">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F97" t="s">
         <v>101</v>

</xml_diff>